<commit_message>
contig stats and figures
</commit_message>
<xml_diff>
--- a/Metagenomic_assembly_analysis/tables/stats for graphs.xlsx
+++ b/Metagenomic_assembly_analysis/tables/stats for graphs.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizabethmallott/Dropbox/Projects/VMI/vmi_hmp/VMI-diet-challenge/Metagenomic_assembly_analysis/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54720745-F87F-A141-A367-3C71043184A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60251C9E-912A-B849-BE3D-2317BFB33862}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="27500" windowHeight="16940" xr2:uid="{F4673523-3607-2E45-B246-EF9DBA27EE5C}"/>
+    <workbookView xWindow="2960" yWindow="500" windowWidth="21980" windowHeight="16940" xr2:uid="{F4673523-3607-2E45-B246-EF9DBA27EE5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="18">
   <si>
     <t>Bray-Curtis</t>
   </si>
@@ -76,6 +76,18 @@
   </si>
   <si>
     <t>TAXONOMY</t>
+  </si>
+  <si>
+    <t>COG</t>
+  </si>
+  <si>
+    <t>ARG</t>
+  </si>
+  <si>
+    <t>Stress</t>
+  </si>
+  <si>
+    <t>CAZymes</t>
   </si>
 </sst>
 </file>
@@ -427,9 +439,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E1D6B9-E1D9-1540-B1D2-9AC16A7036F3}">
-  <dimension ref="A1:O16"/>
+  <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="L57" sqref="L57"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -455,6 +469,9 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
       <c r="F4" t="s">
         <v>9</v>
       </c>
@@ -474,6 +491,9 @@
       </c>
       <c r="C5" t="s">
         <v>12</v>
+      </c>
+      <c r="D5">
+        <v>0.124</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
@@ -513,6 +533,9 @@
       <c r="C6">
         <v>0.126</v>
       </c>
+      <c r="D6">
+        <v>6.5</v>
+      </c>
       <c r="E6" t="s">
         <v>7</v>
       </c>
@@ -745,6 +768,644 @@
       </c>
       <c r="C16">
         <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="I20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" t="s">
+        <v>9</v>
+      </c>
+      <c r="J21" t="s">
+        <v>6</v>
+      </c>
+      <c r="N21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="C22">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="D22">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="G22">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="I22" t="s">
+        <v>2</v>
+      </c>
+      <c r="J22">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="K22">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="M22" t="s">
+        <v>2</v>
+      </c>
+      <c r="N22">
+        <v>1.9E-2</v>
+      </c>
+      <c r="O22">
+        <v>0.46200000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="C23">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="E23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="G23">
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="I23" t="s">
+        <v>3</v>
+      </c>
+      <c r="J23">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="K23">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="M23" t="s">
+        <v>7</v>
+      </c>
+      <c r="N23">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="O23">
+        <v>0.41699999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24">
+        <v>1.6E-2</v>
+      </c>
+      <c r="C24">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="E24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="G24">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="I24" t="s">
+        <v>5</v>
+      </c>
+      <c r="J24">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="K24">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="M24" t="s">
+        <v>8</v>
+      </c>
+      <c r="N24">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="O24">
+        <v>0.63800000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="C25">
+        <v>0.35599999999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" t="s">
+        <v>9</v>
+      </c>
+      <c r="J29" t="s">
+        <v>6</v>
+      </c>
+      <c r="N29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="C30">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="E30" t="s">
+        <v>2</v>
+      </c>
+      <c r="F30">
+        <v>1.9E-2</v>
+      </c>
+      <c r="G30">
+        <v>0.374</v>
+      </c>
+      <c r="I30" t="s">
+        <v>2</v>
+      </c>
+      <c r="J30">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="K30">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="M30" t="s">
+        <v>2</v>
+      </c>
+      <c r="N30">
+        <v>1.9E-2</v>
+      </c>
+      <c r="O30">
+        <v>0.54500000000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="C31">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="E31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31">
+        <v>1.2E-2</v>
+      </c>
+      <c r="G31">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="I31" t="s">
+        <v>3</v>
+      </c>
+      <c r="J31">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="K31">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="M31" t="s">
+        <v>7</v>
+      </c>
+      <c r="N31">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="O31">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32">
+        <v>1.6E-2</v>
+      </c>
+      <c r="C32">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="E32" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="G32">
+        <v>0.23699999999999999</v>
+      </c>
+      <c r="I32" t="s">
+        <v>5</v>
+      </c>
+      <c r="J32">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="K32">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="M32" t="s">
+        <v>8</v>
+      </c>
+      <c r="N32">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="O32">
+        <v>0.72099999999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="C33">
+        <v>0.33300000000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>1</v>
+      </c>
+      <c r="I38" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39" t="s">
+        <v>9</v>
+      </c>
+      <c r="J39" t="s">
+        <v>6</v>
+      </c>
+      <c r="N39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="C40">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="D40">
+        <v>0.06</v>
+      </c>
+      <c r="E40" t="s">
+        <v>2</v>
+      </c>
+      <c r="I40" t="s">
+        <v>2</v>
+      </c>
+      <c r="J40">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="K40">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="M40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C41">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="E41" t="s">
+        <v>7</v>
+      </c>
+      <c r="I41" t="s">
+        <v>3</v>
+      </c>
+      <c r="J41">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="K41">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="M41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C42">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="E42" t="s">
+        <v>8</v>
+      </c>
+      <c r="I42" t="s">
+        <v>5</v>
+      </c>
+      <c r="J42">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="K42">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="M42" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43">
+        <v>1.2E-2</v>
+      </c>
+      <c r="C43">
+        <v>0.82199999999999995</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>10</v>
+      </c>
+      <c r="I45" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>6</v>
+      </c>
+      <c r="F47" t="s">
+        <v>9</v>
+      </c>
+      <c r="J47" t="s">
+        <v>6</v>
+      </c>
+      <c r="N47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="C48">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="E48" t="s">
+        <v>2</v>
+      </c>
+      <c r="I48" t="s">
+        <v>2</v>
+      </c>
+      <c r="J48">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="K48">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="M48" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C49">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="E49" t="s">
+        <v>7</v>
+      </c>
+      <c r="I49" t="s">
+        <v>3</v>
+      </c>
+      <c r="J49">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="K49">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="M49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C50">
+        <v>0.67700000000000005</v>
+      </c>
+      <c r="E50" t="s">
+        <v>8</v>
+      </c>
+      <c r="I50" t="s">
+        <v>5</v>
+      </c>
+      <c r="J50">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="K50">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="M50" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51">
+        <v>1.2E-2</v>
+      </c>
+      <c r="C51">
+        <v>0.82499999999999996</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>1</v>
+      </c>
+      <c r="I55" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" t="s">
+        <v>16</v>
+      </c>
+      <c r="F56" t="s">
+        <v>9</v>
+      </c>
+      <c r="J56" t="s">
+        <v>6</v>
+      </c>
+      <c r="L56" t="s">
+        <v>16</v>
+      </c>
+      <c r="N56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>2</v>
+      </c>
+      <c r="B57">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="C57">
+        <v>0.154</v>
+      </c>
+      <c r="D57">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="E57" t="s">
+        <v>2</v>
+      </c>
+      <c r="I57" t="s">
+        <v>2</v>
+      </c>
+      <c r="J57">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="K57">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="L57">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="M57" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>